<commit_message>
v6.41: changes according to README.md
Update 6.4 from TheDIYGuy999. Added trailer control.
</commit_message>
<xml_diff>
--- a/adjustmentsRemote.xlsx
+++ b/adjustmentsRemote.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10914"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/MacData/Users/martinsommer/Documents/Programmieren/GitHub/RC/Rc_Engine_Sound_ESP32/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Angel\Desktop\Rc_Engine_Sound_ESP32\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9912A7E-D1A5-1E4E-A04E-F143FF72D0AE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2140" yWindow="1380" windowWidth="46720" windowHeight="24940" xr2:uid="{7FD8C6E5-3068-1C47-BC39-03FF60370E8F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11865"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Tabelle1!$E:$U</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="101">
   <si>
     <t>up</t>
   </si>
@@ -235,29 +234,6 @@
   </si>
   <si>
     <t>Micro RC (WLTOYS pistol grip housing, connect it in SBUS communication mode)</t>
-  </si>
-  <si>
-    <r>
-      <t>5th wheel unlocking (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Textkörper)_x0000_"/>
-      </rPr>
-      <t>res</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
   </si>
   <si>
     <t>not available (Switch A internally used for DR)</t>
@@ -408,11 +384,37 @@
       <t>Note, that the PPM input was moved to the "RX" header</t>
     </r>
   </si>
+  <si>
+    <t>Transmission neutral / Trailer control (CH5 &amp;CH6)</t>
+  </si>
+  <si>
+    <r>
+      <t>5th wheel unlocking (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Textkörper)_x0000_"/>
+      </rPr>
+      <t>trailer servo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4">
     <font>
       <sz val="12"/>
@@ -668,6 +670,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -728,6 +739,15 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -785,27 +805,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1165,120 +1167,120 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{796B3C39-3C14-FD4F-A09A-C89C5D5A8330}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:U44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="M44" sqref="M44"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="125" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="M21" sqref="M21:N21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" customWidth="1"/>
+    <col min="1" max="1" width="5.625" customWidth="1"/>
     <col min="2" max="2" width="5" customWidth="1"/>
-    <col min="3" max="3" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.1640625" customWidth="1"/>
-    <col min="6" max="6" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.83203125" customWidth="1"/>
+    <col min="3" max="3" width="5.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.125" customWidth="1"/>
+    <col min="6" max="6" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.875" customWidth="1"/>
     <col min="8" max="8" width="1" customWidth="1"/>
     <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="1" customWidth="1"/>
     <col min="16" max="16" width="8" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="21" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="22.125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="45"/>
-      <c r="I1" s="20" t="s">
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="51"/>
+      <c r="I1" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="P1" s="32" t="s">
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="P1" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
-      <c r="T1" s="32"/>
-      <c r="U1" s="32"/>
+      <c r="Q1" s="35"/>
+      <c r="R1" s="35"/>
+      <c r="S1" s="35"/>
+      <c r="T1" s="35"/>
+      <c r="U1" s="35"/>
     </row>
     <row r="2" spans="1:21">
-      <c r="A2" s="43" t="s">
-        <v>87</v>
-      </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="23" t="s">
+      <c r="A2" s="49" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" s="34"/>
+      <c r="P2" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q2" s="34"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="34"/>
+      <c r="T2" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="U2" s="34"/>
+    </row>
+    <row r="3" spans="1:21" ht="32.1" customHeight="1">
+      <c r="A3" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="B3" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E3" s="27"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="27"/>
+      <c r="I3" s="10" t="s">
         <v>78</v>
-      </c>
-      <c r="G2" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="N2" s="31"/>
-      <c r="P2" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q2" s="31"/>
-      <c r="R2" s="31"/>
-      <c r="S2" s="31"/>
-      <c r="T2" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="U2" s="31"/>
-    </row>
-    <row r="3" spans="1:21" ht="32" customHeight="1">
-      <c r="A3" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="E3" s="24"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="24"/>
-      <c r="I3" s="10" t="s">
-        <v>79</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>17</v>
@@ -1296,7 +1298,7 @@
         <v>26</v>
       </c>
       <c r="P3" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="Q3" s="2" t="s">
         <v>17</v>
@@ -1315,19 +1317,19 @@
       </c>
     </row>
     <row r="4" spans="1:21">
-      <c r="A4" s="46" t="s">
-        <v>80</v>
-      </c>
-      <c r="B4" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="C4" s="46" t="s">
-        <v>77</v>
-      </c>
-      <c r="D4" s="46" t="s">
-        <v>88</v>
-      </c>
-      <c r="E4" s="36" t="s">
+      <c r="A4" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="52" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" s="52" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" s="52" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" s="39" t="s">
         <v>56</v>
       </c>
       <c r="F4" s="11">
@@ -1362,11 +1364,11 @@
       <c r="U4" s="15"/>
     </row>
     <row r="5" spans="1:21">
-      <c r="A5" s="46"/>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="36"/>
+      <c r="A5" s="52"/>
+      <c r="B5" s="52"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="39"/>
       <c r="F5" s="11">
         <v>2</v>
       </c>
@@ -1399,11 +1401,11 @@
       <c r="U5" s="15"/>
     </row>
     <row r="6" spans="1:21">
-      <c r="A6" s="46"/>
-      <c r="B6" s="46"/>
-      <c r="C6" s="46"/>
-      <c r="D6" s="46"/>
-      <c r="E6" s="36"/>
+      <c r="A6" s="52"/>
+      <c r="B6" s="52"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="39"/>
       <c r="F6" s="11">
         <v>3</v>
       </c>
@@ -1436,11 +1438,11 @@
       <c r="U6" s="15"/>
     </row>
     <row r="7" spans="1:21">
-      <c r="A7" s="46"/>
-      <c r="B7" s="46"/>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="36"/>
+      <c r="A7" s="52"/>
+      <c r="B7" s="52"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="39"/>
       <c r="F7" s="11">
         <v>4</v>
       </c>
@@ -1473,21 +1475,21 @@
       <c r="U7" s="15"/>
     </row>
     <row r="8" spans="1:21">
-      <c r="A8" s="46"/>
-      <c r="B8" s="46"/>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="25">
+      <c r="A8" s="52"/>
+      <c r="B8" s="52"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="28">
         <v>5</v>
       </c>
-      <c r="G8" s="28" t="s">
+      <c r="G8" s="31" t="s">
         <v>36</v>
       </c>
       <c r="I8" s="17">
         <v>2</v>
       </c>
-      <c r="J8" s="59" t="s">
+      <c r="J8" s="20" t="s">
         <v>19</v>
       </c>
       <c r="K8" s="18" t="s">
@@ -1505,8 +1507,8 @@
       <c r="P8" s="17">
         <v>4</v>
       </c>
-      <c r="Q8" s="59" t="s">
-        <v>84</v>
+      <c r="Q8" s="20" t="s">
+        <v>83</v>
       </c>
       <c r="R8" s="18" t="s">
         <v>12</v>
@@ -1522,15 +1524,15 @@
       </c>
     </row>
     <row r="9" spans="1:21">
-      <c r="A9" s="46"/>
-      <c r="B9" s="46"/>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="29"/>
+      <c r="A9" s="52"/>
+      <c r="B9" s="52"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="32"/>
       <c r="I9" s="17"/>
-      <c r="J9" s="60"/>
+      <c r="J9" s="21"/>
       <c r="K9" s="18"/>
       <c r="L9" s="1" t="s">
         <v>6</v>
@@ -1538,7 +1540,7 @@
       <c r="M9" s="1"/>
       <c r="N9" s="19"/>
       <c r="P9" s="17"/>
-      <c r="Q9" s="60"/>
+      <c r="Q9" s="21"/>
       <c r="R9" s="18"/>
       <c r="S9" s="1" t="s">
         <v>6</v>
@@ -1547,15 +1549,15 @@
       <c r="U9" s="19"/>
     </row>
     <row r="10" spans="1:21">
-      <c r="A10" s="46"/>
-      <c r="B10" s="46"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="29"/>
+      <c r="A10" s="52"/>
+      <c r="B10" s="52"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="32"/>
       <c r="I10" s="17"/>
-      <c r="J10" s="60"/>
+      <c r="J10" s="21"/>
       <c r="K10" s="18"/>
       <c r="L10" s="1" t="s">
         <v>7</v>
@@ -1565,7 +1567,7 @@
       </c>
       <c r="N10" s="19"/>
       <c r="P10" s="17"/>
-      <c r="Q10" s="60"/>
+      <c r="Q10" s="21"/>
       <c r="R10" s="18"/>
       <c r="S10" s="1" t="s">
         <v>7</v>
@@ -1576,15 +1578,15 @@
       <c r="U10" s="19"/>
     </row>
     <row r="11" spans="1:21">
-      <c r="A11" s="46"/>
-      <c r="B11" s="46"/>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="29"/>
+      <c r="A11" s="52"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="32"/>
       <c r="I11" s="17"/>
-      <c r="J11" s="60"/>
+      <c r="J11" s="21"/>
       <c r="K11" s="18" t="s">
         <v>1</v>
       </c>
@@ -1592,13 +1594,13 @@
         <v>5</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N11" s="1" t="s">
         <v>10</v>
       </c>
       <c r="P11" s="17"/>
-      <c r="Q11" s="60"/>
+      <c r="Q11" s="21"/>
       <c r="R11" s="18" t="s">
         <v>13</v>
       </c>
@@ -1606,22 +1608,22 @@
         <v>5</v>
       </c>
       <c r="T11" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="U11" s="8" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:21">
-      <c r="A12" s="46"/>
-      <c r="B12" s="46"/>
-      <c r="C12" s="46"/>
-      <c r="D12" s="46"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="29"/>
+      <c r="A12" s="52"/>
+      <c r="B12" s="52"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="32"/>
       <c r="I12" s="17"/>
-      <c r="J12" s="60"/>
+      <c r="J12" s="21"/>
       <c r="K12" s="18"/>
       <c r="L12" s="1" t="s">
         <v>6</v>
@@ -1629,7 +1631,7 @@
       <c r="M12" s="1"/>
       <c r="N12" s="19"/>
       <c r="P12" s="17"/>
-      <c r="Q12" s="60"/>
+      <c r="Q12" s="21"/>
       <c r="R12" s="18"/>
       <c r="S12" s="1" t="s">
         <v>6</v>
@@ -1638,15 +1640,15 @@
       <c r="U12" s="19"/>
     </row>
     <row r="13" spans="1:21">
-      <c r="A13" s="46"/>
-      <c r="B13" s="46"/>
-      <c r="C13" s="46"/>
-      <c r="D13" s="46"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="30"/>
+      <c r="A13" s="52"/>
+      <c r="B13" s="52"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="33"/>
       <c r="I13" s="17"/>
-      <c r="J13" s="61"/>
+      <c r="J13" s="22"/>
       <c r="K13" s="18"/>
       <c r="L13" s="1" t="s">
         <v>7</v>
@@ -1656,7 +1658,7 @@
       </c>
       <c r="N13" s="19"/>
       <c r="P13" s="17"/>
-      <c r="Q13" s="61"/>
+      <c r="Q13" s="22"/>
       <c r="R13" s="18"/>
       <c r="S13" s="1" t="s">
         <v>7</v>
@@ -1667,21 +1669,21 @@
       <c r="U13" s="19"/>
     </row>
     <row r="14" spans="1:21">
-      <c r="A14" s="46"/>
-      <c r="B14" s="46"/>
-      <c r="C14" s="46"/>
-      <c r="D14" s="46"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="25">
+      <c r="A14" s="52"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="52"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="28">
         <v>6</v>
       </c>
-      <c r="G14" s="28" t="s">
+      <c r="G14" s="31" t="s">
         <v>37</v>
       </c>
       <c r="I14" s="17">
         <v>4</v>
       </c>
-      <c r="J14" s="59" t="s">
+      <c r="J14" s="20" t="s">
         <v>20</v>
       </c>
       <c r="K14" s="18" t="s">
@@ -1694,11 +1696,11 @@
       <c r="N14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P14" s="39">
+      <c r="P14" s="42">
         <v>16</v>
       </c>
-      <c r="Q14" s="62"/>
-      <c r="R14" s="39"/>
+      <c r="Q14" s="43"/>
+      <c r="R14" s="42"/>
       <c r="S14" s="6" t="s">
         <v>5</v>
       </c>
@@ -1706,15 +1708,15 @@
       <c r="U14" s="6"/>
     </row>
     <row r="15" spans="1:21">
-      <c r="A15" s="46"/>
-      <c r="B15" s="46"/>
-      <c r="C15" s="46"/>
-      <c r="D15" s="46"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="29"/>
+      <c r="A15" s="52"/>
+      <c r="B15" s="52"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="32"/>
       <c r="I15" s="17"/>
-      <c r="J15" s="60"/>
+      <c r="J15" s="21"/>
       <c r="K15" s="18"/>
       <c r="L15" s="1" t="s">
         <v>6</v>
@@ -1723,50 +1725,50 @@
         <v>15</v>
       </c>
       <c r="N15" s="19"/>
-      <c r="P15" s="39"/>
-      <c r="Q15" s="63"/>
-      <c r="R15" s="39"/>
+      <c r="P15" s="42"/>
+      <c r="Q15" s="44"/>
+      <c r="R15" s="42"/>
       <c r="S15" s="6" t="s">
         <v>6</v>
       </c>
       <c r="T15" s="6"/>
-      <c r="U15" s="40"/>
+      <c r="U15" s="46"/>
     </row>
     <row r="16" spans="1:21">
-      <c r="A16" s="46"/>
-      <c r="B16" s="46"/>
-      <c r="C16" s="46"/>
-      <c r="D16" s="46"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="29"/>
+      <c r="A16" s="52"/>
+      <c r="B16" s="52"/>
+      <c r="C16" s="52"/>
+      <c r="D16" s="52"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="32"/>
       <c r="I16" s="17"/>
-      <c r="J16" s="60"/>
+      <c r="J16" s="21"/>
       <c r="K16" s="18"/>
       <c r="L16" s="1" t="s">
         <v>7</v>
       </c>
       <c r="M16" s="1"/>
       <c r="N16" s="19"/>
-      <c r="P16" s="39"/>
-      <c r="Q16" s="63"/>
-      <c r="R16" s="39"/>
+      <c r="P16" s="42"/>
+      <c r="Q16" s="44"/>
+      <c r="R16" s="42"/>
       <c r="S16" s="6" t="s">
         <v>7</v>
       </c>
       <c r="T16" s="6"/>
-      <c r="U16" s="40"/>
+      <c r="U16" s="46"/>
     </row>
     <row r="17" spans="1:21">
-      <c r="A17" s="46"/>
-      <c r="B17" s="46"/>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="29"/>
+      <c r="A17" s="52"/>
+      <c r="B17" s="52"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="32"/>
       <c r="I17" s="17"/>
-      <c r="J17" s="60"/>
+      <c r="J17" s="21"/>
       <c r="K17" s="18" t="s">
         <v>13</v>
       </c>
@@ -1775,11 +1777,11 @@
       </c>
       <c r="M17" s="1"/>
       <c r="N17" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="P17" s="39"/>
-      <c r="Q17" s="63"/>
-      <c r="R17" s="39"/>
+        <v>100</v>
+      </c>
+      <c r="P17" s="42"/>
+      <c r="Q17" s="44"/>
+      <c r="R17" s="42"/>
       <c r="S17" s="6" t="s">
         <v>5</v>
       </c>
@@ -1787,15 +1789,15 @@
       <c r="U17" s="6"/>
     </row>
     <row r="18" spans="1:21">
-      <c r="A18" s="46"/>
-      <c r="B18" s="46"/>
-      <c r="C18" s="46"/>
-      <c r="D18" s="46"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="29"/>
+      <c r="A18" s="52"/>
+      <c r="B18" s="52"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="32"/>
       <c r="I18" s="17"/>
-      <c r="J18" s="60"/>
+      <c r="J18" s="21"/>
       <c r="K18" s="18"/>
       <c r="L18" s="1" t="s">
         <v>6</v>
@@ -1804,53 +1806,53 @@
         <v>16</v>
       </c>
       <c r="N18" s="19"/>
-      <c r="P18" s="39"/>
-      <c r="Q18" s="63"/>
-      <c r="R18" s="39"/>
+      <c r="P18" s="42"/>
+      <c r="Q18" s="44"/>
+      <c r="R18" s="42"/>
       <c r="S18" s="6" t="s">
         <v>6</v>
       </c>
       <c r="T18" s="6"/>
-      <c r="U18" s="40"/>
+      <c r="U18" s="46"/>
     </row>
     <row r="19" spans="1:21">
-      <c r="A19" s="46"/>
-      <c r="B19" s="46"/>
-      <c r="C19" s="46"/>
-      <c r="D19" s="46"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="30"/>
+      <c r="A19" s="52"/>
+      <c r="B19" s="52"/>
+      <c r="C19" s="52"/>
+      <c r="D19" s="52"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="33"/>
       <c r="I19" s="17"/>
-      <c r="J19" s="61"/>
+      <c r="J19" s="22"/>
       <c r="K19" s="18"/>
       <c r="L19" s="1" t="s">
         <v>7</v>
       </c>
       <c r="M19" s="1"/>
       <c r="N19" s="19"/>
-      <c r="P19" s="39"/>
-      <c r="Q19" s="64"/>
-      <c r="R19" s="39"/>
+      <c r="P19" s="42"/>
+      <c r="Q19" s="45"/>
+      <c r="R19" s="42"/>
       <c r="S19" s="6" t="s">
         <v>7</v>
       </c>
       <c r="T19" s="6"/>
-      <c r="U19" s="40"/>
+      <c r="U19" s="46"/>
     </row>
     <row r="20" spans="1:21">
-      <c r="A20" s="47" t="s">
-        <v>89</v>
-      </c>
-      <c r="B20" s="46"/>
-      <c r="C20" s="46"/>
-      <c r="D20" s="46"/>
-      <c r="E20" s="36"/>
+      <c r="A20" s="53" t="s">
+        <v>88</v>
+      </c>
+      <c r="B20" s="52"/>
+      <c r="C20" s="52"/>
+      <c r="D20" s="52"/>
+      <c r="E20" s="39"/>
       <c r="F20" s="11">
         <v>7</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I20" s="4">
         <v>8</v>
@@ -1861,7 +1863,7 @@
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N20" s="16"/>
       <c r="P20" s="7">
@@ -1870,17 +1872,17 @@
       <c r="Q20" s="6"/>
       <c r="R20" s="6"/>
       <c r="S20" s="6"/>
-      <c r="T20" s="33" t="s">
+      <c r="T20" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="U20" s="33"/>
-    </row>
-    <row r="21" spans="1:21" ht="16" customHeight="1">
-      <c r="A21" s="48"/>
-      <c r="B21" s="46"/>
-      <c r="C21" s="46"/>
-      <c r="D21" s="46"/>
-      <c r="E21" s="37" t="s">
+      <c r="U20" s="36"/>
+    </row>
+    <row r="21" spans="1:21" ht="15.95" customHeight="1">
+      <c r="A21" s="54"/>
+      <c r="B21" s="52"/>
+      <c r="C21" s="52"/>
+      <c r="D21" s="52"/>
+      <c r="E21" s="40" t="s">
         <v>59</v>
       </c>
       <c r="F21" s="11">
@@ -1898,7 +1900,7 @@
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="15" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="N21" s="15"/>
       <c r="P21" s="4">
@@ -1910,18 +1912,18 @@
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
       <c r="T21" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="U21" s="15"/>
     </row>
     <row r="22" spans="1:21">
-      <c r="A22" s="48"/>
-      <c r="B22" s="47" t="s">
-        <v>89</v>
-      </c>
-      <c r="C22" s="46"/>
-      <c r="D22" s="46"/>
-      <c r="E22" s="38"/>
+      <c r="A22" s="54"/>
+      <c r="B22" s="53" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" s="52"/>
+      <c r="D22" s="52"/>
+      <c r="E22" s="41"/>
       <c r="F22" s="11">
         <v>9</v>
       </c>
@@ -1936,10 +1938,10 @@
       </c>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
-      <c r="M22" s="34" t="s">
-        <v>92</v>
-      </c>
-      <c r="N22" s="35"/>
+      <c r="M22" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="N22" s="38"/>
       <c r="P22" s="4">
         <v>7</v>
       </c>
@@ -1948,16 +1950,16 @@
       </c>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
-      <c r="T22" s="34" t="s">
-        <v>92</v>
-      </c>
-      <c r="U22" s="35"/>
-    </row>
-    <row r="23" spans="1:21" ht="17">
-      <c r="A23" s="48"/>
-      <c r="B23" s="48"/>
-      <c r="C23" s="46"/>
-      <c r="D23" s="46"/>
+      <c r="T22" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="U22" s="38"/>
+    </row>
+    <row r="23" spans="1:21">
+      <c r="A23" s="54"/>
+      <c r="B23" s="54"/>
+      <c r="C23" s="52"/>
+      <c r="D23" s="52"/>
       <c r="E23" s="12" t="s">
         <v>7</v>
       </c>
@@ -1973,10 +1975,10 @@
       <c r="J23" s="6"/>
       <c r="K23" s="6"/>
       <c r="L23" s="6"/>
-      <c r="M23" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="N23" s="33"/>
+      <c r="M23" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="N23" s="36"/>
       <c r="P23" s="4">
         <v>8</v>
       </c>
@@ -1985,17 +1987,17 @@
       </c>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
-      <c r="T23" s="34" t="s">
+      <c r="T23" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="U23" s="35"/>
+      <c r="U23" s="38"/>
     </row>
     <row r="24" spans="1:21">
-      <c r="A24" s="48"/>
-      <c r="B24" s="48"/>
-      <c r="C24" s="46"/>
-      <c r="D24" s="46"/>
-      <c r="E24" s="50" t="s">
+      <c r="A24" s="54"/>
+      <c r="B24" s="54"/>
+      <c r="C24" s="52"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="56" t="s">
         <v>57</v>
       </c>
       <c r="F24" s="11">
@@ -2010,10 +2012,10 @@
       <c r="J24" s="6"/>
       <c r="K24" s="6"/>
       <c r="L24" s="6"/>
-      <c r="M24" s="33" t="s">
+      <c r="M24" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="N24" s="33"/>
+      <c r="N24" s="36"/>
       <c r="P24" s="4">
         <v>9</v>
       </c>
@@ -2022,17 +2024,17 @@
       </c>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
-      <c r="T24" s="34" t="s">
+      <c r="T24" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="U24" s="35"/>
+      <c r="U24" s="38"/>
     </row>
     <row r="25" spans="1:21">
-      <c r="A25" s="48"/>
-      <c r="B25" s="48"/>
-      <c r="C25" s="46"/>
-      <c r="D25" s="46"/>
-      <c r="E25" s="51"/>
+      <c r="A25" s="54"/>
+      <c r="B25" s="54"/>
+      <c r="C25" s="52"/>
+      <c r="D25" s="52"/>
+      <c r="E25" s="57"/>
       <c r="F25" s="11">
         <v>12</v>
       </c>
@@ -2045,10 +2047,10 @@
       <c r="J25" s="6"/>
       <c r="K25" s="6"/>
       <c r="L25" s="6"/>
-      <c r="M25" s="33" t="s">
+      <c r="M25" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="N25" s="33"/>
+      <c r="N25" s="36"/>
       <c r="P25" s="4">
         <v>10</v>
       </c>
@@ -2057,17 +2059,17 @@
       </c>
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
-      <c r="T25" s="41" t="s">
+      <c r="T25" s="47" t="s">
         <v>62</v>
       </c>
-      <c r="U25" s="42"/>
+      <c r="U25" s="48"/>
     </row>
     <row r="26" spans="1:21">
-      <c r="A26" s="49"/>
-      <c r="B26" s="48"/>
-      <c r="C26" s="46"/>
-      <c r="D26" s="46"/>
-      <c r="E26" s="52"/>
+      <c r="A26" s="55"/>
+      <c r="B26" s="54"/>
+      <c r="C26" s="52"/>
+      <c r="D26" s="52"/>
+      <c r="E26" s="58"/>
       <c r="F26" s="11">
         <v>13</v>
       </c>
@@ -2080,10 +2082,10 @@
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
       <c r="L26" s="6"/>
-      <c r="M26" s="33" t="s">
+      <c r="M26" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="N26" s="33"/>
+      <c r="N26" s="36"/>
       <c r="P26" s="4">
         <v>11</v>
       </c>
@@ -2092,191 +2094,191 @@
       </c>
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
-      <c r="T26" s="41" t="s">
+      <c r="T26" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="U26" s="42"/>
+      <c r="U26" s="48"/>
     </row>
     <row r="28" spans="1:21">
-      <c r="A28" s="55" t="s">
+      <c r="A28" s="61" t="s">
+        <v>81</v>
+      </c>
+      <c r="B28" s="61"/>
+      <c r="C28" s="61"/>
+      <c r="D28" s="61"/>
+      <c r="E28" s="61"/>
+      <c r="F28" s="61"/>
+      <c r="G28" s="61"/>
+      <c r="I28" s="60" t="s">
+        <v>70</v>
+      </c>
+      <c r="J28" s="60"/>
+      <c r="K28" s="60"/>
+      <c r="L28" s="60"/>
+      <c r="M28" s="60"/>
+      <c r="N28" s="60"/>
+      <c r="P28" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21">
+      <c r="A29" s="62" t="s">
+        <v>80</v>
+      </c>
+      <c r="B29" s="62"/>
+      <c r="C29" s="62"/>
+      <c r="D29" s="62"/>
+      <c r="E29" s="62"/>
+      <c r="F29" s="62"/>
+      <c r="G29" s="62"/>
+      <c r="I29" s="59" t="s">
         <v>82</v>
       </c>
-      <c r="B28" s="55"/>
-      <c r="C28" s="55"/>
-      <c r="D28" s="55"/>
-      <c r="E28" s="55"/>
-      <c r="F28" s="55"/>
-      <c r="G28" s="55"/>
-      <c r="I28" s="54" t="s">
-        <v>71</v>
-      </c>
-      <c r="J28" s="54"/>
-      <c r="K28" s="54"/>
-      <c r="L28" s="54"/>
-      <c r="M28" s="54"/>
-      <c r="N28" s="54"/>
-      <c r="P28" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21">
-      <c r="A29" s="56" t="s">
-        <v>81</v>
-      </c>
-      <c r="B29" s="56"/>
-      <c r="C29" s="56"/>
-      <c r="D29" s="56"/>
-      <c r="E29" s="56"/>
-      <c r="F29" s="56"/>
-      <c r="G29" s="56"/>
-      <c r="I29" s="53" t="s">
-        <v>83</v>
-      </c>
-      <c r="J29" s="54"/>
-      <c r="K29" s="54"/>
-      <c r="L29" s="54"/>
-      <c r="M29" s="54"/>
-      <c r="N29" s="54"/>
+      <c r="J29" s="60"/>
+      <c r="K29" s="60"/>
+      <c r="L29" s="60"/>
+      <c r="M29" s="60"/>
+      <c r="N29" s="60"/>
     </row>
     <row r="30" spans="1:21">
-      <c r="A30" s="57" t="s">
-        <v>93</v>
-      </c>
-      <c r="B30" s="57"/>
-      <c r="C30" s="57"/>
-      <c r="D30" s="57"/>
-      <c r="E30" s="57"/>
-      <c r="F30" s="57"/>
-      <c r="G30" s="57"/>
-      <c r="I30" s="54"/>
-      <c r="J30" s="54"/>
-      <c r="K30" s="54"/>
-      <c r="L30" s="54"/>
-      <c r="M30" s="54"/>
-      <c r="N30" s="54"/>
-    </row>
-    <row r="31" spans="1:21" ht="16" customHeight="1">
-      <c r="I31" s="58" t="s">
+      <c r="A30" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="B30" s="63"/>
+      <c r="C30" s="63"/>
+      <c r="D30" s="63"/>
+      <c r="E30" s="63"/>
+      <c r="F30" s="63"/>
+      <c r="G30" s="63"/>
+      <c r="I30" s="60"/>
+      <c r="J30" s="60"/>
+      <c r="K30" s="60"/>
+      <c r="L30" s="60"/>
+      <c r="M30" s="60"/>
+      <c r="N30" s="60"/>
+    </row>
+    <row r="31" spans="1:21" ht="15.95" customHeight="1">
+      <c r="I31" s="64" t="s">
+        <v>97</v>
+      </c>
+      <c r="J31" s="64"/>
+      <c r="K31" s="64"/>
+      <c r="L31" s="64"/>
+      <c r="M31" s="64"/>
+      <c r="N31" s="64"/>
+    </row>
+    <row r="32" spans="1:21" ht="15.95" customHeight="1">
+      <c r="A32" s="64" t="s">
         <v>98</v>
       </c>
-      <c r="J31" s="58"/>
-      <c r="K31" s="58"/>
-      <c r="L31" s="58"/>
-      <c r="M31" s="58"/>
-      <c r="N31" s="58"/>
-    </row>
-    <row r="32" spans="1:21" ht="16" customHeight="1">
-      <c r="A32" s="58" t="s">
-        <v>99</v>
-      </c>
-      <c r="B32" s="58"/>
-      <c r="C32" s="58"/>
-      <c r="D32" s="58"/>
-      <c r="E32" s="58"/>
-      <c r="F32" s="58"/>
-      <c r="G32" s="58"/>
-      <c r="I32" s="58"/>
-      <c r="J32" s="58"/>
-      <c r="K32" s="58"/>
-      <c r="L32" s="58"/>
-      <c r="M32" s="58"/>
-      <c r="N32" s="58"/>
-    </row>
-    <row r="33" spans="1:14" ht="16" customHeight="1">
-      <c r="A33" s="58"/>
-      <c r="B33" s="58"/>
-      <c r="C33" s="58"/>
-      <c r="D33" s="58"/>
-      <c r="E33" s="58"/>
-      <c r="F33" s="58"/>
-      <c r="G33" s="58"/>
-      <c r="I33" s="58"/>
-      <c r="J33" s="58"/>
-      <c r="K33" s="58"/>
-      <c r="L33" s="58"/>
-      <c r="M33" s="58"/>
-      <c r="N33" s="58"/>
-    </row>
-    <row r="34" spans="1:14" ht="16" customHeight="1">
-      <c r="A34" s="58"/>
-      <c r="B34" s="58"/>
-      <c r="C34" s="58"/>
-      <c r="D34" s="58"/>
-      <c r="E34" s="58"/>
-      <c r="F34" s="58"/>
-      <c r="G34" s="58"/>
-      <c r="I34" s="58" t="s">
-        <v>85</v>
-      </c>
-      <c r="J34" s="58"/>
-      <c r="K34" s="58"/>
-      <c r="L34" s="58"/>
-      <c r="M34" s="58"/>
-      <c r="N34" s="58"/>
+      <c r="B32" s="64"/>
+      <c r="C32" s="64"/>
+      <c r="D32" s="64"/>
+      <c r="E32" s="64"/>
+      <c r="F32" s="64"/>
+      <c r="G32" s="64"/>
+      <c r="I32" s="64"/>
+      <c r="J32" s="64"/>
+      <c r="K32" s="64"/>
+      <c r="L32" s="64"/>
+      <c r="M32" s="64"/>
+      <c r="N32" s="64"/>
+    </row>
+    <row r="33" spans="1:14" ht="15.95" customHeight="1">
+      <c r="A33" s="64"/>
+      <c r="B33" s="64"/>
+      <c r="C33" s="64"/>
+      <c r="D33" s="64"/>
+      <c r="E33" s="64"/>
+      <c r="F33" s="64"/>
+      <c r="G33" s="64"/>
+      <c r="I33" s="64"/>
+      <c r="J33" s="64"/>
+      <c r="K33" s="64"/>
+      <c r="L33" s="64"/>
+      <c r="M33" s="64"/>
+      <c r="N33" s="64"/>
+    </row>
+    <row r="34" spans="1:14" ht="15.95" customHeight="1">
+      <c r="A34" s="64"/>
+      <c r="B34" s="64"/>
+      <c r="C34" s="64"/>
+      <c r="D34" s="64"/>
+      <c r="E34" s="64"/>
+      <c r="F34" s="64"/>
+      <c r="G34" s="64"/>
+      <c r="I34" s="64" t="s">
+        <v>84</v>
+      </c>
+      <c r="J34" s="64"/>
+      <c r="K34" s="64"/>
+      <c r="L34" s="64"/>
+      <c r="M34" s="64"/>
+      <c r="N34" s="64"/>
     </row>
     <row r="35" spans="1:14">
-      <c r="A35" s="58"/>
-      <c r="B35" s="58"/>
-      <c r="C35" s="58"/>
-      <c r="D35" s="58"/>
-      <c r="E35" s="58"/>
-      <c r="F35" s="58"/>
-      <c r="G35" s="58"/>
-      <c r="I35" s="58"/>
-      <c r="J35" s="58"/>
-      <c r="K35" s="58"/>
-      <c r="L35" s="58"/>
-      <c r="M35" s="58"/>
-      <c r="N35" s="58"/>
+      <c r="A35" s="64"/>
+      <c r="B35" s="64"/>
+      <c r="C35" s="64"/>
+      <c r="D35" s="64"/>
+      <c r="E35" s="64"/>
+      <c r="F35" s="64"/>
+      <c r="G35" s="64"/>
+      <c r="I35" s="64"/>
+      <c r="J35" s="64"/>
+      <c r="K35" s="64"/>
+      <c r="L35" s="64"/>
+      <c r="M35" s="64"/>
+      <c r="N35" s="64"/>
     </row>
     <row r="36" spans="1:14">
-      <c r="A36" s="58"/>
-      <c r="B36" s="58"/>
-      <c r="C36" s="58"/>
-      <c r="D36" s="58"/>
-      <c r="E36" s="58"/>
-      <c r="F36" s="58"/>
-      <c r="G36" s="58"/>
-      <c r="I36" s="54" t="s">
-        <v>95</v>
-      </c>
-      <c r="J36" s="54"/>
-      <c r="K36" s="54"/>
-      <c r="L36" s="54"/>
-      <c r="M36" s="54"/>
-      <c r="N36" s="54"/>
+      <c r="A36" s="64"/>
+      <c r="B36" s="64"/>
+      <c r="C36" s="64"/>
+      <c r="D36" s="64"/>
+      <c r="E36" s="64"/>
+      <c r="F36" s="64"/>
+      <c r="G36" s="64"/>
+      <c r="I36" s="60" t="s">
+        <v>94</v>
+      </c>
+      <c r="J36" s="60"/>
+      <c r="K36" s="60"/>
+      <c r="L36" s="60"/>
+      <c r="M36" s="60"/>
+      <c r="N36" s="60"/>
     </row>
     <row r="37" spans="1:14">
-      <c r="A37" s="58"/>
-      <c r="B37" s="58"/>
-      <c r="C37" s="58"/>
-      <c r="D37" s="58"/>
-      <c r="E37" s="58"/>
-      <c r="F37" s="58"/>
-      <c r="G37" s="58"/>
-      <c r="I37" s="53" t="s">
-        <v>97</v>
-      </c>
-      <c r="J37" s="53"/>
-      <c r="K37" s="53"/>
-      <c r="L37" s="53"/>
-      <c r="M37" s="53"/>
-      <c r="N37" s="53"/>
+      <c r="A37" s="64"/>
+      <c r="B37" s="64"/>
+      <c r="C37" s="64"/>
+      <c r="D37" s="64"/>
+      <c r="E37" s="64"/>
+      <c r="F37" s="64"/>
+      <c r="G37" s="64"/>
+      <c r="I37" s="59" t="s">
+        <v>96</v>
+      </c>
+      <c r="J37" s="59"/>
+      <c r="K37" s="59"/>
+      <c r="L37" s="59"/>
+      <c r="M37" s="59"/>
+      <c r="N37" s="59"/>
     </row>
     <row r="38" spans="1:14">
-      <c r="A38" s="58"/>
-      <c r="B38" s="58"/>
-      <c r="C38" s="58"/>
-      <c r="D38" s="58"/>
-      <c r="E38" s="58"/>
-      <c r="F38" s="58"/>
-      <c r="G38" s="58"/>
-      <c r="I38" s="53"/>
-      <c r="J38" s="53"/>
-      <c r="K38" s="53"/>
-      <c r="L38" s="53"/>
-      <c r="M38" s="53"/>
-      <c r="N38" s="53"/>
+      <c r="A38" s="64"/>
+      <c r="B38" s="64"/>
+      <c r="C38" s="64"/>
+      <c r="D38" s="64"/>
+      <c r="E38" s="64"/>
+      <c r="F38" s="64"/>
+      <c r="G38" s="64"/>
+      <c r="I38" s="59"/>
+      <c r="J38" s="59"/>
+      <c r="K38" s="59"/>
+      <c r="L38" s="59"/>
+      <c r="M38" s="59"/>
+      <c r="N38" s="59"/>
     </row>
     <row r="39" spans="1:14">
       <c r="A39" s="13"/>

</xml_diff>